<commit_message>
Change seed data passwords according to rules, create passwords from the .xlsx file then seeding data, make hashing public static method in account service
</commit_message>
<xml_diff>
--- a/Persistence/Database/test_data/Couriers.xlsx
+++ b/Persistence/Database/test_data/Couriers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieva\Desktop\PSK\komandinis\shipping-service\Persistence\Database\test-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vieva\Desktop\PSK\komandinis\shipping-service\Persistence\Database\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2253BA-F944-4C60-8B93-4F2E60593B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936E96BC-E92D-4171-96D0-77B861B5ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16951523-755D-4673-83F3-901F0B7B3088}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{16951523-755D-4673-83F3-901F0B7B3088}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -109,31 +109,34 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Kebabas</t>
-  </si>
-  <si>
-    <t>Pieštukas17</t>
-  </si>
-  <si>
-    <t>Lėktuvas23</t>
-  </si>
-  <si>
-    <t>Zebras33</t>
-  </si>
-  <si>
-    <t>ABC!!23</t>
-  </si>
-  <si>
-    <t>ABC??12</t>
-  </si>
-  <si>
-    <t>ErelisLėktuve</t>
-  </si>
-  <si>
-    <t>Sparnuotas</t>
-  </si>
-  <si>
-    <t>ABCCAB</t>
+    <t>Kebabas13!</t>
+  </si>
+  <si>
+    <t>Pieštukas17!</t>
+  </si>
+  <si>
+    <t>Lėktuvas23!</t>
+  </si>
+  <si>
+    <t>Zebras33!</t>
+  </si>
+  <si>
+    <t>ABC!!23??a</t>
+  </si>
+  <si>
+    <t>ABC??12aa</t>
+  </si>
+  <si>
+    <t>ErelisLėktuve!i2</t>
+  </si>
+  <si>
+    <t>Sparnuotas?O2?</t>
+  </si>
+  <si>
+    <t>125521ABCa??</t>
+  </si>
+  <si>
+    <t>ABCCABa1??</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,8 +643,8 @@
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1">
-        <v>125521</v>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
@@ -655,7 +658,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>21</v>

</xml_diff>